<commit_message>
New plots and paper versions 4 and 5
</commit_message>
<xml_diff>
--- a/Model/Sensi Runs/2016-01 sensi runs/variable_impact.xlsx
+++ b/Model/Sensi Runs/2016-01 sensi runs/variable_impact.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="% impact (2)" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="52">
   <si>
     <t>PV_incentive</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">PV cust: huge positive boost from efficiency improvement.  Neg impact from req'd rate of return. Smaller neg impact from util fixed cost and wholesale price and debt interest rate. </t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -572,6 +575,8 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,8 +619,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1511,8 +1514,8 @@
   <dimension ref="A1:BD38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A18" sqref="A18"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1527,70 +1530,70 @@
       </c>
     </row>
     <row r="2" spans="1:49" ht="16" thickTop="1">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="59" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="59" t="s">
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="59" t="s">
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="59" t="s">
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="59" t="s">
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="59" t="s">
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="59" t="s">
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="61"/>
-      <c r="AH2" s="59" t="s">
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="61"/>
-      <c r="AL2" s="62" t="s">
+      <c r="AI2" s="62"/>
+      <c r="AJ2" s="62"/>
+      <c r="AK2" s="63"/>
+      <c r="AL2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="64"/>
-      <c r="AP2" s="65"/>
-      <c r="AQ2" s="65"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="66"/>
+      <c r="AP2" s="67"/>
+      <c r="AQ2" s="67"/>
+      <c r="AR2" s="67"/>
+      <c r="AS2" s="67"/>
       <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
@@ -1717,650 +1720,650 @@
       <c r="AO3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
     </row>
     <row r="4" spans="1:49">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="7">
-        <v>-0.70801136887537197</v>
+        <v>-0.70727143207738397</v>
       </c>
       <c r="C4" s="4">
-        <v>1.33872944070016</v>
+        <v>1.37767015048913</v>
       </c>
       <c r="D4" s="4">
-        <v>-5.0234329967315396</v>
+        <v>-5.1047297471237201</v>
       </c>
       <c r="E4" s="8">
-        <v>0.31456199473260399</v>
+        <v>0.31580397087721701</v>
       </c>
       <c r="F4" s="7">
-        <v>-7.2329023344822998E-3</v>
+        <v>-7.2664785030246599E-3</v>
       </c>
       <c r="G4" s="4">
-        <v>-5.30633587170583</v>
+        <v>-6.0094445544428501</v>
       </c>
       <c r="H4" s="4">
-        <v>15.959154933585999</v>
+        <v>16.7972928711362</v>
       </c>
       <c r="I4" s="4">
-        <v>-0.156963696609346</v>
+        <v>-0.17432792834628899</v>
       </c>
       <c r="J4" s="7">
-        <v>-5.6485439392819101</v>
+        <v>-5.6474285144921099</v>
       </c>
       <c r="K4" s="4">
-        <v>-9.0040135672216692</v>
+        <v>-10.1058833006852</v>
       </c>
       <c r="L4" s="4">
-        <v>45.657054029257701</v>
+        <v>46.193893044124401</v>
       </c>
       <c r="M4" s="4">
-        <v>1.9826774472173101</v>
+        <v>1.9587297013962801</v>
       </c>
       <c r="N4" s="7">
-        <v>-1.4314898996463701</v>
+        <v>-1.43183130106264</v>
       </c>
       <c r="O4" s="4">
-        <v>-5.2942580361067497</v>
+        <v>-6.5724132217715203</v>
       </c>
       <c r="P4" s="4">
-        <v>8.4714415723489793</v>
+        <v>8.9978957805039705</v>
       </c>
       <c r="Q4" s="4">
-        <v>0.39570873921976402</v>
+        <v>0.36751107523680199</v>
       </c>
       <c r="R4" s="7">
-        <v>-0.77759277245848102</v>
+        <v>-0.77716316497334204</v>
       </c>
       <c r="S4" s="4">
-        <v>44.922147071202197</v>
+        <v>55.1989333769992</v>
       </c>
       <c r="T4" s="4">
-        <v>-37.9083891799757</v>
+        <v>-38.398521122798499</v>
       </c>
       <c r="U4" s="4">
-        <v>42.779276509749899</v>
+        <v>42.9160223257825</v>
       </c>
       <c r="V4" s="7">
-        <v>-1.6171232966056801</v>
+        <v>-1.62278367846177</v>
       </c>
       <c r="W4" s="4">
-        <v>-11.161612188605901</v>
+        <v>-12.598930568008299</v>
       </c>
       <c r="X4" s="4">
-        <v>47.124399947056901</v>
+        <v>49.621407966245201</v>
       </c>
       <c r="Y4" s="8">
-        <v>49.379749054126201</v>
+        <v>49.655166238173699</v>
       </c>
       <c r="Z4" s="7">
-        <v>-2.25924209088573</v>
+        <v>-2.2501089750458698</v>
       </c>
       <c r="AA4" s="4">
-        <v>-11.0396542431646</v>
+        <v>-12.296146007280599</v>
       </c>
       <c r="AB4" s="4">
-        <v>51.627416535148001</v>
+        <v>53.988952312423301</v>
       </c>
       <c r="AC4" s="8">
-        <v>54.708698230328899</v>
+        <v>54.14986767557</v>
       </c>
       <c r="AD4" s="7">
-        <v>-9.2081010471227701E-2</v>
+        <v>-9.1904470678438502E-2</v>
       </c>
       <c r="AE4" s="4">
-        <v>-7.8530709567963104</v>
+        <v>-8.7301665480115407</v>
       </c>
       <c r="AF4" s="4">
-        <v>35.172483280101901</v>
+        <v>36.889972767334903</v>
       </c>
       <c r="AG4" s="8">
-        <v>-0.21379891930564199</v>
+        <v>-0.23710731354811601</v>
       </c>
       <c r="AH4" s="7">
-        <v>-1.4563036375606801E-2</v>
+        <v>-1.4601341268146601E-2</v>
       </c>
       <c r="AI4" s="4">
-        <v>-0.391601871708331</v>
+        <v>-0.30891653570609001</v>
       </c>
       <c r="AJ4" s="4">
-        <v>5.3583538805749598</v>
+        <v>5.7250384693193599</v>
       </c>
       <c r="AK4" s="8">
-        <v>-7.63911473896215E-3</v>
+        <v>-7.9751169786109605E-3</v>
       </c>
       <c r="AL4" s="7">
-        <v>-3.2169493694474101</v>
+        <v>-3.2159045004983899</v>
       </c>
       <c r="AM4" s="4">
-        <v>-18.122907258095999</v>
+        <v>-20.132627932523199</v>
       </c>
       <c r="AN4" s="4">
-        <v>106.41268181785701</v>
+        <v>113.129900409352</v>
       </c>
       <c r="AO4" s="8">
-        <v>0.66664594875838101</v>
-      </c>
-      <c r="AP4" s="65"/>
-      <c r="AQ4" s="65"/>
-      <c r="AR4" s="65"/>
-      <c r="AS4" s="65"/>
+        <v>0.60920237004293598</v>
+      </c>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67"/>
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
     </row>
     <row r="5" spans="1:49">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7">
-        <v>-0.60372488914988898</v>
+        <v>-0.60404817068251104</v>
       </c>
       <c r="C5" s="4">
-        <v>1.1724170788797701</v>
+        <v>1.1823959928513601</v>
       </c>
       <c r="D5" s="4">
-        <v>-3.5357974017866001</v>
+        <v>-3.5070431917831901</v>
       </c>
       <c r="E5" s="8">
-        <v>0.39796751705007199</v>
+        <v>0.39694902458459502</v>
       </c>
       <c r="F5" s="7">
-        <v>1.40459259994245E-3</v>
+        <v>3.3318819320821797E-4</v>
       </c>
       <c r="G5" s="4">
-        <v>-5.31555178284981</v>
+        <v>-3.7519027408933101</v>
       </c>
       <c r="H5" s="4">
-        <v>11.0145544920747</v>
+        <v>10.2781692275656</v>
       </c>
       <c r="I5" s="4">
-        <v>-0.32425341430057097</v>
+        <v>-0.26393568333844097</v>
       </c>
       <c r="J5" s="7">
-        <v>-5.90459271983491</v>
+        <v>-5.9092482110940603</v>
       </c>
       <c r="K5" s="4">
-        <v>-4.9098093639209202</v>
+        <v>-2.3288826128702098</v>
       </c>
       <c r="L5" s="4">
-        <v>34.995849536740003</v>
+        <v>32.472338847096601</v>
       </c>
       <c r="M5" s="4">
-        <v>2.6224091371668599</v>
+        <v>2.7693505178743498</v>
       </c>
       <c r="N5" s="7">
-        <v>-0.76550776994014003</v>
+        <v>-0.76722368204758695</v>
       </c>
       <c r="O5" s="4">
-        <v>-5.32181924026409</v>
+        <v>-2.42181158051531</v>
       </c>
       <c r="P5" s="4">
-        <v>5.4595216089192604</v>
+        <v>4.4077753782305296</v>
       </c>
       <c r="Q5" s="4">
-        <v>0.15925681170400899</v>
+        <v>0.26683106558345898</v>
       </c>
       <c r="R5" s="7">
-        <v>-1.1034434184278601</v>
+        <v>-1.09930272743831</v>
       </c>
       <c r="S5" s="4">
-        <v>311.84419513653802</v>
+        <v>24.558524846755901</v>
       </c>
       <c r="T5" s="4">
-        <v>-24.511535565896502</v>
+        <v>-23.8194801805091</v>
       </c>
       <c r="U5" s="4">
-        <v>56.437247877942298</v>
+        <v>56.103156094987099</v>
       </c>
       <c r="V5" s="7">
-        <v>-1.86843704651801</v>
+        <v>-1.86728404681505</v>
       </c>
       <c r="W5" s="4">
-        <v>-9.8174673730505209</v>
+        <v>-7.09486656965489</v>
       </c>
       <c r="X5" s="4">
-        <v>43.115722743096498</v>
+        <v>40.304821755993302</v>
       </c>
       <c r="Y5" s="8">
-        <v>52.908943988957503</v>
+        <v>52.807281066245899</v>
       </c>
       <c r="Z5" s="7">
-        <v>-1.9747023624570199</v>
+        <v>-1.98327616912586</v>
       </c>
       <c r="AA5" s="4">
-        <v>-8.1793503327663597</v>
+        <v>-5.4815197949185102</v>
       </c>
       <c r="AB5" s="4">
-        <v>31.839668389147</v>
+        <v>29.566479509370801</v>
       </c>
       <c r="AC5" s="8">
-        <v>39.4561502347795</v>
+        <v>39.967278315642801</v>
       </c>
       <c r="AD5" s="7">
-        <v>-0.21973117101477799</v>
+        <v>-0.22158508881021499</v>
       </c>
       <c r="AE5" s="4">
-        <v>-7.7018277824560997</v>
+        <v>-5.8238931198505099</v>
       </c>
       <c r="AF5" s="4">
-        <v>29.455305268871101</v>
+        <v>27.9884489063692</v>
       </c>
       <c r="AG5" s="8">
-        <v>-0.45150896761142501</v>
+        <v>-0.370507059517932</v>
       </c>
       <c r="AH5" s="7">
-        <v>-5.3237470779649201E-2</v>
+        <v>-5.4077423271755597E-2</v>
       </c>
       <c r="AI5" s="4">
-        <v>3.47174747414652</v>
+        <v>-0.77090920654856498</v>
       </c>
       <c r="AJ5" s="4">
-        <v>6.9075635533497</v>
+        <v>6.4331389194612401</v>
       </c>
       <c r="AK5" s="8">
-        <v>-7.2222669399925193E-2</v>
+        <v>-4.8428830442556699E-2</v>
       </c>
       <c r="AL5" s="7">
-        <v>-3.3722249840849301</v>
+        <v>-3.3779795506868702</v>
       </c>
       <c r="AM5" s="4">
-        <v>-11.568614056568</v>
+        <v>-8.8186740440253999</v>
       </c>
       <c r="AN5" s="4">
-        <v>73.492929726702002</v>
+        <v>66.056244134818201</v>
       </c>
       <c r="AO5" s="8">
-        <v>0.75302012874142699</v>
-      </c>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="65"/>
-      <c r="AR5" s="65"/>
-      <c r="AS5" s="65"/>
+        <v>0.99249215103189903</v>
+      </c>
+      <c r="AP5" s="67"/>
+      <c r="AQ5" s="67"/>
+      <c r="AR5" s="67"/>
+      <c r="AS5" s="67"/>
     </row>
     <row r="6" spans="1:49">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="7">
-        <v>-1.2169398237970499</v>
+        <v>-1.2167507619114899</v>
       </c>
       <c r="C6" s="4">
-        <v>2.62972082724569</v>
+        <v>2.5649849990813198</v>
       </c>
       <c r="D6" s="4">
-        <v>-2.1993400162532502</v>
+        <v>-2.1442796745739701</v>
       </c>
       <c r="E6" s="8">
-        <v>0.87107416590116005</v>
+        <v>0.86482943205278995</v>
       </c>
       <c r="F6" s="7">
-        <v>8.1684891741095993E-3</v>
+        <v>6.3216348807457797E-3</v>
       </c>
       <c r="G6" s="4">
-        <v>-6.7778075613767204</v>
+        <v>-6.0537744832803702</v>
       </c>
       <c r="H6" s="4">
-        <v>12.655679408091</v>
+        <v>12.3135719178789</v>
       </c>
       <c r="I6" s="4">
-        <v>-0.96218735173290704</v>
+        <v>-0.905681528846082</v>
       </c>
       <c r="J6" s="7">
-        <v>-6.1917190865332898</v>
+        <v>-6.1938617540353498</v>
       </c>
       <c r="K6" s="4">
-        <v>-1.1150954683427301</v>
+        <v>-0.30457239721693202</v>
       </c>
       <c r="L6" s="4">
-        <v>20.261695213425799</v>
+        <v>19.7363649474662</v>
       </c>
       <c r="M6" s="4">
-        <v>2.48528431164062</v>
+        <v>2.5663101323076201</v>
       </c>
       <c r="N6" s="7">
-        <v>-1.0238349711728301</v>
+        <v>-1.0257583561822701</v>
       </c>
       <c r="O6" s="4">
-        <v>-2.9838738719654598</v>
+        <v>-2.09682890908568</v>
       </c>
       <c r="P6" s="4">
-        <v>4.8527847786175302</v>
+        <v>4.4438771223308997</v>
       </c>
       <c r="Q6" s="4">
-        <v>0.171601901377091</v>
+        <v>0.244268132532871</v>
       </c>
       <c r="R6" s="7">
-        <v>-1.3697870834822901</v>
+        <v>-1.3667294232950999</v>
       </c>
       <c r="S6" s="4">
-        <v>29.4759050069426</v>
+        <v>21.346403062251898</v>
       </c>
       <c r="T6" s="4">
-        <v>-18.222266337140901</v>
+        <v>-17.894227627260701</v>
       </c>
       <c r="U6" s="4">
-        <v>61.721836240287999</v>
+        <v>61.518969493874103</v>
       </c>
       <c r="V6" s="7">
-        <v>-1.8684559617758101</v>
+        <v>-1.86979707219577</v>
       </c>
       <c r="W6" s="4">
-        <v>-5.5448800948126298</v>
+        <v>-4.7067543775722198</v>
       </c>
       <c r="X6" s="4">
-        <v>15.810852429625999</v>
+        <v>15.388578297172799</v>
       </c>
       <c r="Y6" s="8">
-        <v>40.102471586519499</v>
+        <v>40.132873237425002</v>
       </c>
       <c r="Z6" s="7">
-        <v>-1.95024063055491</v>
+        <v>-1.95345689342613</v>
       </c>
       <c r="AA6" s="4">
-        <v>-3.7049652577174998</v>
+        <v>-2.9020045684262601</v>
       </c>
       <c r="AB6" s="4">
-        <v>10.8919792464776</v>
+        <v>10.4769850932563</v>
       </c>
       <c r="AC6" s="8">
-        <v>33.325654811295301</v>
+        <v>33.491356441738397</v>
       </c>
       <c r="AD6" s="7">
-        <v>-0.19556642839466401</v>
+        <v>-0.19700934603162601</v>
       </c>
       <c r="AE6" s="4">
-        <v>-5.2651212576777597</v>
+        <v>-4.7341706575158398</v>
       </c>
       <c r="AF6" s="4">
-        <v>11.4426822782907</v>
+        <v>11.1652165401276</v>
       </c>
       <c r="AG6" s="8">
-        <v>-0.72062548857583597</v>
+        <v>-0.67673246564970801</v>
       </c>
       <c r="AH6" s="7">
-        <v>-3.5115991817337301E-2</v>
+        <v>-3.56543130826752E-2</v>
       </c>
       <c r="AI6" s="4">
-        <v>-0.72551242431676</v>
+        <v>-0.53746276416330896</v>
       </c>
       <c r="AJ6" s="4">
-        <v>1.6345254160653599</v>
+        <v>1.5442162066317899</v>
       </c>
       <c r="AK6" s="8">
-        <v>-9.5286611383760503E-2</v>
+        <v>-7.9469105069555096E-2</v>
       </c>
       <c r="AL6" s="7">
-        <v>-3.6431015704556802</v>
+        <v>-3.64672989002815</v>
       </c>
       <c r="AM6" s="4">
-        <v>-6.82421159021313</v>
+        <v>-5.8896091007315796</v>
       </c>
       <c r="AN6" s="4">
-        <v>26.8549893986334</v>
+        <v>25.762438036876301</v>
       </c>
       <c r="AO6" s="8">
-        <v>0.58586780779931102</v>
-      </c>
-      <c r="AP6" s="65"/>
-      <c r="AQ6" s="65"/>
-      <c r="AR6" s="65"/>
-      <c r="AS6" s="65"/>
+        <v>0.711236945074741</v>
+      </c>
+      <c r="AP6" s="67"/>
+      <c r="AQ6" s="67"/>
+      <c r="AR6" s="67"/>
+      <c r="AS6" s="67"/>
     </row>
     <row r="7" spans="1:49">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="7">
-        <v>-0.59428327556233995</v>
+        <v>-0.594283949659414</v>
       </c>
       <c r="C7" s="4">
-        <v>1.4613340626901301</v>
+        <v>1.46169349348377</v>
       </c>
       <c r="D7" s="4">
-        <v>-4.98098609816505</v>
+        <v>-4.9819024925797102</v>
       </c>
       <c r="E7" s="8">
-        <v>0.39227048019039301</v>
+        <v>0.39229475551029303</v>
       </c>
       <c r="F7" s="7">
-        <v>-5.8963733398156399E-3</v>
+        <v>-5.8900130623870698E-3</v>
       </c>
       <c r="G7" s="4">
-        <v>-0.188588210983379</v>
+        <v>-0.192991003246891</v>
       </c>
       <c r="H7" s="4">
-        <v>1.33888337671824</v>
+        <v>1.3679095544394899</v>
       </c>
       <c r="I7" s="4">
-        <v>-1.32348492117442E-2</v>
+        <v>-1.3556865830969799E-2</v>
       </c>
       <c r="J7" s="7">
-        <v>-4.92988128680215</v>
+        <v>-4.9298794020090302</v>
       </c>
       <c r="K7" s="4">
-        <v>5.3548406843579501</v>
+        <v>5.3514934063075703</v>
       </c>
       <c r="L7" s="4">
-        <v>6.1331574473566297</v>
+        <v>6.1471081582701501</v>
       </c>
       <c r="M7" s="4">
-        <v>2.6286271129748502</v>
+        <v>2.6283991186922999</v>
       </c>
       <c r="N7" s="7">
-        <v>-1.35984602520301</v>
+        <v>-1.3598453115828499</v>
       </c>
       <c r="O7" s="4">
-        <v>1.79325609566514</v>
+        <v>1.79283992392183</v>
       </c>
       <c r="P7" s="4">
-        <v>-0.92595777659081302</v>
+        <v>-0.92551123833883697</v>
       </c>
       <c r="Q7" s="4">
-        <v>0.751623434786448</v>
+        <v>0.75160052730417204</v>
       </c>
       <c r="R7" s="7">
-        <v>-1.56735153310256</v>
+        <v>-1.5673582635763299</v>
       </c>
       <c r="S7" s="4">
-        <v>3.4926315719516698</v>
+        <v>3.4991357525391402</v>
       </c>
       <c r="T7" s="4">
-        <v>-9.3035578802433001</v>
+        <v>-9.3105219013216605</v>
       </c>
       <c r="U7" s="4">
-        <v>53.996410818846499</v>
+        <v>53.996854492384003</v>
       </c>
       <c r="V7" s="7">
-        <v>-2.1588612986052902</v>
+        <v>-2.15885514308812</v>
       </c>
       <c r="W7" s="4">
-        <v>1.89834775535987</v>
+        <v>1.8939950111169599</v>
       </c>
       <c r="X7" s="4">
-        <v>4.9468201851910703</v>
+        <v>4.9758083502892898</v>
       </c>
       <c r="Y7" s="8">
-        <v>47.057046505027301</v>
+        <v>47.056667291443702</v>
       </c>
       <c r="Z7" s="7">
-        <v>-2.1860933336744401</v>
+        <v>-2.18608671392027</v>
       </c>
       <c r="AA7" s="4">
-        <v>1.76853970850371</v>
+        <v>1.7641123399640799</v>
       </c>
       <c r="AB7" s="4">
-        <v>6.57612584906704</v>
+        <v>6.6123514613682497</v>
       </c>
       <c r="AC7" s="8">
-        <v>46.2032994220028</v>
+        <v>46.2027547467993</v>
       </c>
       <c r="AD7" s="7">
-        <v>-0.19668827678891901</v>
+        <v>-0.19668287758452299</v>
       </c>
       <c r="AE7" s="4">
-        <v>-0.99459913599267402</v>
+        <v>-0.99822266320670106</v>
       </c>
       <c r="AF7" s="4">
-        <v>9.9006269681198908</v>
+        <v>9.9245253651766401</v>
       </c>
       <c r="AG7" s="8">
-        <v>-2.7548316098308798E-2</v>
+        <v>-2.78114376558391E-2</v>
       </c>
       <c r="AH7" s="7">
-        <v>-3.0752172040745599E-2</v>
+        <v>-3.0751557563542999E-2</v>
       </c>
       <c r="AI7" s="4">
-        <v>-9.2509751311499494E-2</v>
+        <v>-9.2931220938072004E-2</v>
       </c>
       <c r="AJ7" s="4">
-        <v>1.4499004837488401</v>
+        <v>1.4538082176920699</v>
       </c>
       <c r="AK7" s="8">
-        <v>3.3196901431859801E-3</v>
+        <v>3.2899980799145699E-3</v>
       </c>
       <c r="AL7" s="7">
-        <v>-4.00616658775132</v>
+        <v>-4.0061601675774101</v>
       </c>
       <c r="AM7" s="4">
-        <v>3.7158241535904999</v>
+        <v>3.71143658761277</v>
       </c>
       <c r="AN7" s="4">
-        <v>10.0961670926437</v>
+        <v>10.1346933904602</v>
       </c>
       <c r="AO7" s="8">
-        <v>2.2588872971049998</v>
-      </c>
-      <c r="AP7" s="65"/>
-      <c r="AQ7" s="65"/>
-      <c r="AR7" s="65"/>
-      <c r="AS7" s="65"/>
+        <v>2.2585617033130401</v>
+      </c>
+      <c r="AP7" s="67"/>
+      <c r="AQ7" s="67"/>
+      <c r="AR7" s="67"/>
+      <c r="AS7" s="67"/>
     </row>
     <row r="8" spans="1:49">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="7">
-        <v>-1.0459261119816501</v>
+        <v>-1.04540328616645</v>
       </c>
       <c r="C8" s="4">
-        <v>1.6994265266103299</v>
+        <v>1.6695905838612699</v>
       </c>
       <c r="D8" s="4">
-        <v>-1.6529985942724801</v>
+        <v>-1.6282879661382601</v>
       </c>
       <c r="E8" s="8">
-        <v>0.61388160590553598</v>
+        <v>0.60765128829521697</v>
       </c>
       <c r="F8" s="7">
-        <v>1.12840269148774E-2</v>
+        <v>8.3233254851000707E-3</v>
       </c>
       <c r="G8" s="4">
-        <v>-12.600147882550299</v>
+        <v>-10.958860453517</v>
       </c>
       <c r="H8" s="4">
-        <v>25.037163128216701</v>
+        <v>24.5624757642133</v>
       </c>
       <c r="I8" s="4">
-        <v>-1.14170372745825</v>
+        <v>-1.0432571317752699</v>
       </c>
       <c r="J8" s="7">
-        <v>-6.7864016340858599</v>
+        <v>-6.7918741325625902</v>
       </c>
       <c r="K8" s="4">
-        <v>-19.0651800283099</v>
+        <v>-16.566387719306501</v>
       </c>
       <c r="L8" s="4">
-        <v>63.854424500956597</v>
+        <v>61.293266905296001</v>
       </c>
       <c r="M8" s="4">
-        <v>1.5875182255240301</v>
+        <v>1.7894067140958501</v>
       </c>
       <c r="N8" s="7">
-        <v>-0.75970785528902895</v>
+        <v>-0.76394169145667701</v>
       </c>
       <c r="O8" s="4">
-        <v>-13.600229511901</v>
+        <v>-10.891386258571901</v>
       </c>
       <c r="P8" s="4">
-        <v>14.8690733554071</v>
+        <v>13.8397742570688</v>
       </c>
       <c r="Q8" s="4">
-        <v>-0.48210613107494898</v>
+        <v>-0.32820590210518902</v>
       </c>
       <c r="R8" s="7">
-        <v>-0.88810099956472599</v>
+        <v>-0.87978749649702204</v>
       </c>
       <c r="S8" s="4">
-        <v>350.81107949475199</v>
+        <v>62.282907036986302</v>
       </c>
       <c r="T8" s="4">
-        <v>-41.229410633071602</v>
+        <v>-40.438728667827597</v>
       </c>
       <c r="U8" s="4">
-        <v>54.104095774701001</v>
+        <v>53.6662050805026</v>
       </c>
       <c r="V8" s="7">
-        <v>-1.7304148997742499</v>
+        <v>-1.73518855845082</v>
       </c>
       <c r="W8" s="4">
-        <v>-20.0338181804211</v>
+        <v>-17.502594635238701</v>
       </c>
       <c r="X8" s="4">
-        <v>55.121722381460103</v>
+        <v>53.575142453212699</v>
       </c>
       <c r="Y8" s="8">
-        <v>48.598032490201902</v>
+        <v>48.711690409728199</v>
       </c>
       <c r="Z8" s="7">
-        <v>-1.60914845849919</v>
+        <v>-1.61393406587013</v>
       </c>
       <c r="AA8" s="4">
-        <v>-20.9422467336111</v>
+        <v>-18.4826695260079</v>
       </c>
       <c r="AB8" s="4">
-        <v>60.097438768982499</v>
+        <v>58.945758318453798</v>
       </c>
       <c r="AC8" s="8">
-        <v>37.644710875360303</v>
+        <v>37.926397379686897</v>
       </c>
       <c r="AD8" s="7">
-        <v>-0.13025320325252701</v>
+        <v>-0.13347440103133101</v>
       </c>
       <c r="AE8" s="4">
-        <v>-14.1530764433783</v>
+        <v>-12.481460556516501</v>
       </c>
       <c r="AF8" s="4">
-        <v>40.404392236625803</v>
+        <v>39.9278642265092</v>
       </c>
       <c r="AG8" s="8">
-        <v>-1.0813610556097399</v>
+        <v>-0.97927847659887501</v>
       </c>
       <c r="AH8" s="7">
-        <v>-3.6299985862722699E-2</v>
+        <v>-3.7712607714834402E-2</v>
       </c>
       <c r="AI8" s="4">
-        <v>3.1215398903555198</v>
+        <v>-0.88718964253436605</v>
       </c>
       <c r="AJ8" s="4">
-        <v>7.317870014765</v>
+        <v>7.0379270981059197</v>
       </c>
       <c r="AK8" s="8">
-        <v>-0.161223508872849</v>
+        <v>-0.123865678138743</v>
       </c>
       <c r="AL8" s="7">
-        <v>-2.8947199667266799</v>
+        <v>-2.9035024090027699</v>
       </c>
       <c r="AM8" s="4">
-        <v>-31.874377333399501</v>
+        <v>-29.679066139358302</v>
       </c>
       <c r="AN8" s="4">
-        <v>133.018421904592</v>
+        <v>129.45331031565999</v>
       </c>
       <c r="AO8" s="8">
-        <v>-1.39741480152866</v>
+        <v>-1.0790940837895</v>
       </c>
     </row>
     <row r="9" spans="1:49">
@@ -2368,124 +2371,124 @@
         <v>16</v>
       </c>
       <c r="B9" s="7">
-        <v>-0.88846669427832503</v>
+        <v>-0.88838312884551596</v>
       </c>
       <c r="C9" s="4">
-        <v>1.9801067575251701</v>
+        <v>1.99376706507678</v>
       </c>
       <c r="D9" s="4">
-        <v>-4.1245857223338502</v>
+        <v>-4.14586215476292</v>
       </c>
       <c r="E9" s="8">
-        <v>0.57745159158790704</v>
+        <v>0.57763638370909298</v>
       </c>
       <c r="F9" s="7">
-        <v>-3.0474741354919901E-3</v>
+        <v>-3.0449678517836601E-3</v>
       </c>
       <c r="G9" s="4">
-        <v>-4.6109591223987199</v>
+        <v>-4.6632703218526101</v>
       </c>
       <c r="H9" s="4">
-        <v>13.2533423288167</v>
+        <v>13.458648697927901</v>
       </c>
       <c r="I9" s="4">
-        <v>-0.28846588597283102</v>
+        <v>-0.28713114292456998</v>
       </c>
       <c r="J9" s="7">
-        <v>-6.0285728247621</v>
+        <v>-6.0287849450498898</v>
       </c>
       <c r="K9" s="4">
-        <v>-1.3185790555334</v>
+        <v>-1.5244439977734101</v>
       </c>
       <c r="L9" s="4">
-        <v>30.927016831110301</v>
+        <v>30.962221775121101</v>
       </c>
       <c r="M9" s="4">
-        <v>2.8742255575259099</v>
+        <v>2.8765845187901098</v>
       </c>
       <c r="N9" s="7">
-        <v>-1.1012787602673</v>
+        <v>-1.10102633625297</v>
       </c>
       <c r="O9" s="4">
-        <v>-1.7929777321004301</v>
+        <v>-1.9925073767224499</v>
       </c>
       <c r="P9" s="4">
-        <v>4.84063238106945</v>
+        <v>4.9352852623354604</v>
       </c>
       <c r="Q9" s="4">
-        <v>0.45705014858936399</v>
+        <v>0.455215648154149</v>
       </c>
       <c r="R9" s="7">
-        <v>-0.79537074170134603</v>
+        <v>-0.79604955563339297</v>
       </c>
       <c r="S9" s="4">
-        <v>31.938536147978599</v>
+        <v>35.321818496481598</v>
       </c>
       <c r="T9" s="4">
-        <v>-30.109222569698101</v>
+        <v>-30.362978361419099</v>
       </c>
       <c r="U9" s="4">
-        <v>52.837854034432603</v>
+        <v>52.875088341757099</v>
       </c>
       <c r="V9" s="7">
-        <v>-1.4647401065199599</v>
+        <v>-1.46582109593365</v>
       </c>
       <c r="W9" s="4">
-        <v>-8.3884892314078598</v>
+        <v>-8.7919518911136905</v>
       </c>
       <c r="X9" s="4">
-        <v>45.982432553128199</v>
+        <v>46.763857215909297</v>
       </c>
       <c r="Y9" s="8">
-        <v>46.7360856343739</v>
+        <v>46.826962840672699</v>
       </c>
       <c r="Z9" s="7">
-        <v>-2.3889432917240399</v>
+        <v>-2.3868212578074499</v>
       </c>
       <c r="AA9" s="4">
-        <v>-3.7502628085410601</v>
+        <v>-3.96111318458148</v>
       </c>
       <c r="AB9" s="4">
-        <v>27.685499552723101</v>
+        <v>28.474307135228301</v>
       </c>
       <c r="AC9" s="8">
-        <v>43.642492979040703</v>
+        <v>43.479350306464902</v>
       </c>
       <c r="AD9" s="7">
-        <v>-0.180437129839224</v>
+        <v>-0.18034162690442501</v>
       </c>
       <c r="AE9" s="4">
-        <v>-5.6723444175592199</v>
+        <v>-5.80854710565466</v>
       </c>
       <c r="AF9" s="4">
-        <v>25.765451622517901</v>
+        <v>26.1912486221458</v>
       </c>
       <c r="AG9" s="8">
-        <v>-0.27702400378485298</v>
+        <v>-0.277256924461043</v>
       </c>
       <c r="AH9" s="7">
-        <v>-3.5864341069124998E-2</v>
+        <v>-3.5868912344199998E-2</v>
       </c>
       <c r="AI9" s="4">
-        <v>-0.67439696092259205</v>
+        <v>-0.63716764294552597</v>
       </c>
       <c r="AJ9" s="4">
-        <v>5.1326723514761898</v>
+        <v>5.2106582796144103</v>
       </c>
       <c r="AK9" s="8">
-        <v>-1.7244576792984499E-2</v>
+        <v>-1.5297372431894701E-2</v>
       </c>
       <c r="AL9" s="7">
-        <v>-3.3313893695100201</v>
+        <v>-3.3309513646332398</v>
       </c>
       <c r="AM9" s="4">
-        <v>-8.3571797250682192</v>
+        <v>-8.87328152553461</v>
       </c>
       <c r="AN9" s="4">
-        <v>63.646011945956801</v>
+        <v>65.360578874926205</v>
       </c>
       <c r="AO9" s="8">
-        <v>1.14406138972278</v>
+        <v>1.1334638466260401</v>
       </c>
     </row>
     <row r="10" spans="1:49" ht="16" thickBot="1">
@@ -2494,163 +2497,163 @@
       </c>
       <c r="B10" s="9">
         <f>AVERAGE(B4:B9)</f>
-        <v>-0.84289202727410428</v>
+        <v>-0.84269012155712752</v>
       </c>
       <c r="C10" s="10">
         <f t="shared" ref="C10:AO10" si="0">AVERAGE(C4:C9)</f>
-        <v>1.7136224489418754</v>
+        <v>1.7083503808072715</v>
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
-        <v>-3.5861901382571282</v>
+        <v>-3.5853508711602946</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>0.52786789256127864</v>
+        <v>0.5258608091715341</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="0"/>
-        <v>7.8005981318992007E-4</v>
+        <v>-2.0388514302355351E-4</v>
       </c>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>-5.7998984053107927</v>
+        <v>-5.2717072595388386</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="0"/>
-        <v>13.209796277917226</v>
+        <v>13.129678005526898</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>-0.48113482088094156</v>
+        <v>-0.44798171351027033</v>
       </c>
       <c r="J10" s="9">
         <f t="shared" si="0"/>
-        <v>-5.9149519152167036</v>
+        <v>-5.9168461598738382</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="0"/>
-        <v>-5.0096394664951118</v>
+        <v>-4.2464461035907801</v>
       </c>
       <c r="L10" s="10">
         <f t="shared" si="0"/>
-        <v>33.638199593141174</v>
+        <v>32.800865612895741</v>
       </c>
       <c r="M10" s="10">
         <f t="shared" si="0"/>
-        <v>2.3634569653415967</v>
+        <v>2.4314634505260853</v>
       </c>
       <c r="N10" s="9">
         <f t="shared" si="0"/>
-        <v>-1.0736108802531132</v>
+        <v>-1.0749377797641655</v>
       </c>
       <c r="O10" s="10">
         <f t="shared" si="0"/>
-        <v>-4.5333170494454311</v>
+        <v>-3.6970179037908384</v>
       </c>
       <c r="P10" s="10">
         <f t="shared" si="0"/>
-        <v>6.2612493199619168</v>
+        <v>5.9498494270218032</v>
       </c>
       <c r="Q10" s="10">
         <f t="shared" si="0"/>
-        <v>0.24218915076695446</v>
+        <v>0.29287009111771062</v>
       </c>
       <c r="R10" s="9">
         <f t="shared" si="0"/>
-        <v>-1.0836077581228771</v>
+        <v>-1.0810651052355829</v>
       </c>
       <c r="S10" s="10">
         <f t="shared" si="0"/>
-        <v>128.74741573822752</v>
+        <v>33.701287095335672</v>
       </c>
       <c r="T10" s="10">
         <f t="shared" si="0"/>
-        <v>-26.88073036100435</v>
+        <v>-26.704076310189446</v>
       </c>
       <c r="U10" s="10">
         <f t="shared" si="0"/>
-        <v>53.646120209326718</v>
+        <v>53.512715971547898</v>
       </c>
       <c r="V10" s="9">
         <f t="shared" si="0"/>
-        <v>-1.7846721016331666</v>
+        <v>-1.78662159915753</v>
       </c>
       <c r="W10" s="10">
         <f t="shared" si="0"/>
-        <v>-8.8413198854896908</v>
+        <v>-8.1335171717451402</v>
       </c>
       <c r="X10" s="10">
         <f t="shared" si="0"/>
-        <v>35.350325039926467</v>
+        <v>35.104936006470432</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="0"/>
-        <v>47.463721543201054</v>
+        <v>47.531773513948202</v>
       </c>
       <c r="Z10" s="9">
         <f t="shared" si="0"/>
-        <v>-2.0613950279658884</v>
+        <v>-2.0622806791992847</v>
       </c>
       <c r="AA10" s="10">
         <f t="shared" si="0"/>
-        <v>-7.641323277882818</v>
+        <v>-6.8932234568751118</v>
       </c>
       <c r="AB10" s="10">
         <f t="shared" si="0"/>
-        <v>31.453021390257543</v>
+        <v>31.344138971683453</v>
       </c>
       <c r="AC10" s="11">
         <f t="shared" si="0"/>
-        <v>42.496834425467917</v>
+        <v>42.536167477650388</v>
       </c>
       <c r="AD10" s="9">
         <f t="shared" si="0"/>
-        <v>-0.16912620329355663</v>
+        <v>-0.1701663018400931</v>
       </c>
       <c r="AE10" s="10">
         <f t="shared" si="0"/>
-        <v>-6.9400066656433923</v>
+        <v>-6.4294101084592912</v>
       </c>
       <c r="AF10" s="10">
         <f t="shared" si="0"/>
-        <v>25.356823609087883</v>
+        <v>25.347879404610556</v>
       </c>
       <c r="AG10" s="11">
         <f t="shared" si="0"/>
-        <v>-0.46197779183096749</v>
+        <v>-0.42811561290525219</v>
       </c>
       <c r="AH10" s="9">
         <f t="shared" si="0"/>
-        <v>-3.4305499657531102E-2</v>
+        <v>-3.4777692540859134E-2</v>
       </c>
       <c r="AI10" s="10">
         <f t="shared" si="0"/>
-        <v>0.78487772604047634</v>
+        <v>-0.53909616880598799</v>
       </c>
       <c r="AJ10" s="10">
         <f t="shared" si="0"/>
-        <v>4.6334809499966747</v>
+        <v>4.5674645318041316</v>
       </c>
       <c r="AK10" s="11">
         <f t="shared" si="0"/>
-        <v>-5.8382798507549231E-2</v>
+        <v>-4.529101749690765E-2</v>
       </c>
       <c r="AL10" s="9">
         <f t="shared" si="0"/>
-        <v>-3.4107586413293398</v>
+        <v>-3.4135379804044717</v>
       </c>
       <c r="AM10" s="10">
         <f t="shared" si="0"/>
-        <v>-12.171910968292394</v>
+        <v>-11.613637025760054</v>
       </c>
       <c r="AN10" s="10">
         <f t="shared" si="0"/>
-        <v>68.920200314397476</v>
+        <v>68.316194193682136</v>
       </c>
       <c r="AO10" s="11">
         <f t="shared" si="0"/>
-        <v>0.66851129509970653</v>
+        <v>0.77097715538319278</v>
       </c>
     </row>
     <row r="11" spans="1:49" ht="16" thickTop="1">
@@ -2696,7 +2699,7 @@
       <c r="AF11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="AI11" s="73"/>
+      <c r="AI11" s="59"/>
       <c r="AL11" s="27" t="s">
         <v>31</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>28</v>
       </c>
       <c r="AC12" s="16"/>
-      <c r="AI12" s="74"/>
+      <c r="AI12" s="60"/>
     </row>
     <row r="13" spans="1:49">
       <c r="H13" t="s">
@@ -2772,40 +2775,40 @@
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="61"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="63"/>
     </row>
     <row r="24" spans="1:56" ht="17" thickTop="1" thickBot="1">
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
     </row>
     <row r="25" spans="1:56" ht="16" thickTop="1">
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
     </row>
     <row r="26" spans="1:56" ht="16" thickBot="1"/>
     <row r="27" spans="1:56" ht="17" thickTop="1" thickBot="1">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
       <c r="F27" s="25" t="s">
         <v>26</v>
       </c>
@@ -2817,18 +2820,18 @@
       </c>
     </row>
     <row r="28" spans="1:56" ht="17" thickTop="1" thickBot="1">
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="59" t="s">
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="61"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="63"/>
       <c r="J28" s="14" t="s">
         <v>27</v>
       </c>
@@ -2847,12 +2850,12 @@
       <c r="R28" s="16"/>
     </row>
     <row r="29" spans="1:56" ht="17" thickTop="1" thickBot="1">
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="61"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="63"/>
       <c r="F29" s="27" t="s">
         <v>31</v>
       </c>
@@ -2864,20 +2867,22 @@
       </c>
     </row>
     <row r="30" spans="1:56" ht="16" thickTop="1">
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
       <c r="F30" s="27" t="s">
         <v>31</v>
       </c>
       <c r="H30" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I30" t="s">
-        <v>34</v>
+    </row>
+    <row r="31" spans="1:56">
+      <c r="I31" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:56">
@@ -4614,72 +4619,72 @@
       </c>
     </row>
     <row r="2" spans="1:49" ht="16" thickTop="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="66" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="66" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="66" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="66" t="s">
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="66" t="s">
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="67"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="68"/>
-      <c r="Z2" s="66" t="s">
+      <c r="W2" s="69"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="66" t="s">
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="68"/>
-      <c r="AH2" s="66" t="s">
+      <c r="AE2" s="69"/>
+      <c r="AF2" s="69"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="67"/>
-      <c r="AJ2" s="67"/>
-      <c r="AK2" s="68"/>
-      <c r="AL2" s="69" t="s">
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="69"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="AM2" s="70"/>
-      <c r="AN2" s="70"/>
-      <c r="AO2" s="71"/>
-      <c r="AP2" s="72" t="s">
+      <c r="AM2" s="72"/>
+      <c r="AN2" s="72"/>
+      <c r="AO2" s="73"/>
+      <c r="AP2" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="AQ2" s="72"/>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="72"/>
+      <c r="AQ2" s="74"/>
+      <c r="AR2" s="74"/>
+      <c r="AS2" s="74"/>
       <c r="AT2" s="34"/>
       <c r="AU2" s="34"/>
       <c r="AV2" s="34"/>
@@ -4806,10 +4811,10 @@
       <c r="AO3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AP3" s="72"/>
-      <c r="AQ3" s="72"/>
-      <c r="AR3" s="72"/>
-      <c r="AS3" s="72"/>
+      <c r="AP3" s="74"/>
+      <c r="AQ3" s="74"/>
+      <c r="AR3" s="74"/>
+      <c r="AS3" s="74"/>
     </row>
     <row r="4" spans="1:49">
       <c r="A4" s="33" t="s">
@@ -4935,10 +4940,10 @@
       <c r="AO4" s="45">
         <v>-0.55715508122564295</v>
       </c>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="72"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="74"/>
     </row>
     <row r="5" spans="1:49">
       <c r="A5" s="33" t="s">
@@ -5064,10 +5069,10 @@
       <c r="AO5" s="45">
         <v>-0.58094455542591406</v>
       </c>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="72"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="74"/>
     </row>
     <row r="6" spans="1:49">
       <c r="A6" s="33" t="s">
@@ -5193,10 +5198,10 @@
       <c r="AO6" s="45">
         <v>-0.45204729754416501</v>
       </c>
-      <c r="AP6" s="72"/>
-      <c r="AQ6" s="72"/>
-      <c r="AR6" s="72"/>
-      <c r="AS6" s="72"/>
+      <c r="AP6" s="74"/>
+      <c r="AQ6" s="74"/>
+      <c r="AR6" s="74"/>
+      <c r="AS6" s="74"/>
     </row>
     <row r="7" spans="1:49">
       <c r="A7" s="33" t="s">
@@ -5322,10 +5327,10 @@
       <c r="AO7" s="45">
         <v>-2.1932974345889402</v>
       </c>
-      <c r="AP7" s="72"/>
-      <c r="AQ7" s="72"/>
-      <c r="AR7" s="72"/>
-      <c r="AS7" s="72"/>
+      <c r="AP7" s="74"/>
+      <c r="AQ7" s="74"/>
+      <c r="AR7" s="74"/>
+      <c r="AS7" s="74"/>
     </row>
     <row r="8" spans="1:49">
       <c r="A8" s="33" t="s">
@@ -5876,40 +5881,40 @@
       <c r="A23" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="70"/>
     </row>
     <row r="24" spans="1:56" ht="17" thickTop="1" thickBot="1">
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
     </row>
     <row r="25" spans="1:56" ht="16" thickTop="1">
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="70"/>
     </row>
     <row r="26" spans="1:56" ht="16" thickBot="1"/>
     <row r="27" spans="1:56" ht="17" thickTop="1" thickBot="1">
       <c r="A27" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="29" t="s">
         <v>26</v>
       </c>
@@ -5921,18 +5926,18 @@
       </c>
     </row>
     <row r="28" spans="1:56" ht="17" thickTop="1" thickBot="1">
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="66" t="s">
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="68"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="70"/>
       <c r="J28" s="52" t="s">
         <v>27</v>
       </c>
@@ -5951,12 +5956,12 @@
       <c r="R28" s="51"/>
     </row>
     <row r="29" spans="1:56" ht="17" thickTop="1" thickBot="1">
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="68"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="70"/>
       <c r="F29" s="50" t="s">
         <v>31</v>
       </c>
@@ -5968,12 +5973,12 @@
       </c>
     </row>
     <row r="30" spans="1:56" ht="16" thickTop="1">
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
       <c r="F30" s="50" t="s">
         <v>31</v>
       </c>

</xml_diff>